<commit_message>
updating excel sheet with test passed/failed.
</commit_message>
<xml_diff>
--- a/bin/data.xlsx
+++ b/bin/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="92">
   <si>
     <t xml:space="preserve">fname</t>
   </si>
@@ -79,25 +79,241 @@
     <t xml:space="preserve">negative</t>
   </si>
   <si>
+    <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-12-1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kalwar Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“240”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajasthan</t>
+  </si>
+  <si>
     <t xml:space="preserve">name</t>
   </si>
   <si>
-    <t xml:space="preserve">12-12-12</t>
+    <t xml:space="preserve">JLN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suneeta Reddy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAL/ETA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09-06-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12-12-1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queens Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“12”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mumbai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maharashtra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sawai Man Singh Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delhi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kewal Krishan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TS/NPS/NS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08-05-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Claire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cruise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-02-2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Connaught Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“A-24”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alwar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blood in EDTA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07-06-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-05-2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“980”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acute Sera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04-06-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jodhpur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">two</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Covalent Sera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05-06-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vijay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plair</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“323”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Udaipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">three</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05-05-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11-11-1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajmer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">four</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B-28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4-05-2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">George</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“34”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bikaner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">five</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3-05-2020</t>
+  </si>
+  <si>
+    <t>Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -157,12 +373,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -183,19 +407,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1:U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="18.2"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="14.44"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="18" style="0" width="11.52"/>
+    <col min="1" max="2" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="3" max="3" customWidth="false" hidden="false" style="1" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="4" max="4" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="5" max="5" customWidth="true" hidden="false" style="2" width="22.92" collapsed="true" outlineLevel="0"/>
+    <col min="6" max="8" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="9" max="9" customWidth="true" hidden="false" style="0" width="21.56" collapsed="true" outlineLevel="0"/>
+    <col min="10" max="10" customWidth="false" hidden="false" style="2" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="11" max="13" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="14" max="14" customWidth="true" hidden="false" style="0" width="18.2" collapsed="true" outlineLevel="0"/>
+    <col min="15" max="15" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="16" max="16" customWidth="true" hidden="false" style="0" width="13.89" collapsed="true" outlineLevel="0"/>
+    <col min="17" max="17" customWidth="true" hidden="false" style="0" width="14.43" collapsed="true" outlineLevel="0"/>
+    <col min="18" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,13 +437,13 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
@@ -226,7 +458,7 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
@@ -262,58 +494,524 @@
         <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" s="1" t="b">
+        <v>29</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O2" s="3" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="S2" s="1" t="b">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="R2" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S2" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="R5" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S5" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="R6" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S6" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O7" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="R7" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S7" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="R8" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S8" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="O9" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="R9" s="3" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="S9" s="3" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="U9" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>